<commit_message>
Got a rough version of the instrument CSV import going, need to refine it a little bit but it is working pretty well so far.
</commit_message>
<xml_diff>
--- a/doc/MSCI Global Industry Classificaction Standard.xlsx
+++ b/doc/MSCI Global Industry Classificaction Standard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Share\Trading\Projects\TradeSharp\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5BCA114-4444-4996-A2BF-22B892102246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{383D5776-38F3-4D60-8E9B-AB55F57D2ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="27736" windowHeight="16395" xr2:uid="{D2974B2A-D996-4834-A8A5-481C6D04C88D}"/>
   </bookViews>
@@ -25,19 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="235">
-  <si>
-    <t>Sector</t>
-  </si>
-  <si>
-    <t>Industry Group</t>
-  </si>
-  <si>
-    <t>Industry</t>
-  </si>
-  <si>
-    <t>Sub-Industry</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="233">
   <si>
     <t>Energy</t>
   </si>
@@ -730,6 +718,12 @@
   </si>
   <si>
     <t>Real Estate Services</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -1084,7 +1078,7 @@
   <dimension ref="A1:H164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D121" sqref="D121"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1099,16 +1093,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>231</v>
+      </c>
+      <c r="B1" t="s">
+        <v>232</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>231</v>
+      </c>
+      <c r="D1" t="s">
+        <v>232</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>231</v>
+      </c>
+      <c r="F1" t="s">
+        <v>232</v>
       </c>
       <c r="G1" t="s">
-        <v>3</v>
+        <v>231</v>
+      </c>
+      <c r="H1" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
@@ -1116,25 +1122,25 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>1010</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <v>101010</v>
       </c>
       <c r="F2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <v>10101010</v>
       </c>
       <c r="H2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
@@ -1142,25 +1148,25 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>1010</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>101010</v>
       </c>
       <c r="F3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <v>10101020</v>
       </c>
       <c r="H3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
@@ -1168,25 +1174,25 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>1010</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E4">
         <v>101020</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G4">
         <v>10102010</v>
       </c>
       <c r="H4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
@@ -1194,25 +1200,25 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>1010</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E5">
         <v>101020</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G5">
         <v>10102020</v>
       </c>
       <c r="H5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
@@ -1220,25 +1226,25 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>1010</v>
       </c>
       <c r="D6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <v>101020</v>
       </c>
       <c r="F6" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G6">
         <v>10102030</v>
       </c>
       <c r="H6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
@@ -1246,25 +1252,25 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <v>1010</v>
       </c>
       <c r="D7" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <v>101020</v>
       </c>
       <c r="F7" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G7">
         <v>10102040</v>
       </c>
       <c r="H7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
@@ -1272,25 +1278,25 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <v>1010</v>
       </c>
       <c r="D8" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E8">
         <v>101020</v>
       </c>
       <c r="F8" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G8">
         <v>10102050</v>
       </c>
       <c r="H8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.45">
@@ -1298,25 +1304,25 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C9">
         <v>1510</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E9">
         <v>151010</v>
       </c>
       <c r="F9" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G9">
         <v>15101010</v>
       </c>
       <c r="H9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.45">
@@ -1324,25 +1330,25 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C10">
         <v>1510</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E10">
         <v>151010</v>
       </c>
       <c r="F10" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G10">
         <v>15101020</v>
       </c>
       <c r="H10" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.45">
@@ -1350,25 +1356,25 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <v>1510</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E11">
         <v>151010</v>
       </c>
       <c r="F11" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G11">
         <v>15101030</v>
       </c>
       <c r="H11" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.45">
@@ -1376,25 +1382,25 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C12">
         <v>1510</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E12">
         <v>151010</v>
       </c>
       <c r="F12" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G12">
         <v>15101040</v>
       </c>
       <c r="H12" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.45">
@@ -1402,25 +1408,25 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C13">
         <v>1510</v>
       </c>
       <c r="D13" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E13">
         <v>151010</v>
       </c>
       <c r="F13" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G13">
         <v>15101050</v>
       </c>
       <c r="H13" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.45">
@@ -1428,25 +1434,25 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C14">
         <v>1510</v>
       </c>
       <c r="D14" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E14">
         <v>151020</v>
       </c>
       <c r="F14" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G14">
         <v>15102010</v>
       </c>
       <c r="H14" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.45">
@@ -1454,25 +1460,25 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C15">
         <v>1510</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E15">
         <v>151030</v>
       </c>
       <c r="F15" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G15">
         <v>15103010</v>
       </c>
       <c r="H15" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.45">
@@ -1480,25 +1486,25 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C16">
         <v>1510</v>
       </c>
       <c r="D16" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E16">
         <v>151030</v>
       </c>
       <c r="F16" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G16">
         <v>15103020</v>
       </c>
       <c r="H16" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.45">
@@ -1506,25 +1512,25 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C17">
         <v>1510</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E17">
         <v>151040</v>
       </c>
       <c r="F17" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G17">
         <v>15104010</v>
       </c>
       <c r="H17" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.45">
@@ -1532,25 +1538,25 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C18">
         <v>1510</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E18">
         <v>151040</v>
       </c>
       <c r="F18" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G18">
         <v>15104020</v>
       </c>
       <c r="H18" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.45">
@@ -1558,25 +1564,25 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C19">
         <v>1510</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E19">
         <v>151040</v>
       </c>
       <c r="F19" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G19">
         <v>15104025</v>
       </c>
       <c r="H19" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.45">
@@ -1584,25 +1590,25 @@
         <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C20">
         <v>1510</v>
       </c>
       <c r="D20" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E20">
         <v>151040</v>
       </c>
       <c r="F20" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G20">
         <v>15104030</v>
       </c>
       <c r="H20" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.45">
@@ -1610,25 +1616,25 @@
         <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C21">
         <v>1510</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E21">
         <v>151040</v>
       </c>
       <c r="F21" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G21">
         <v>15104040</v>
       </c>
       <c r="H21" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.45">
@@ -1636,25 +1642,25 @@
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C22">
         <v>1510</v>
       </c>
       <c r="D22" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E22">
         <v>151040</v>
       </c>
       <c r="F22" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G22">
         <v>15104045</v>
       </c>
       <c r="H22" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.45">
@@ -1662,25 +1668,25 @@
         <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C23">
         <v>1510</v>
       </c>
       <c r="D23" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E23">
         <v>151040</v>
       </c>
       <c r="F23" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G23">
         <v>15104050</v>
       </c>
       <c r="H23" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.45">
@@ -1688,25 +1694,25 @@
         <v>15</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C24">
         <v>1510</v>
       </c>
       <c r="D24" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E24">
         <v>151050</v>
       </c>
       <c r="F24" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G24">
         <v>15105010</v>
       </c>
       <c r="H24" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.45">
@@ -1714,25 +1720,25 @@
         <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C25">
         <v>1510</v>
       </c>
       <c r="D25" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E25">
         <v>151050</v>
       </c>
       <c r="F25" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G25">
         <v>15105020</v>
       </c>
       <c r="H25" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.45">
@@ -1740,25 +1746,25 @@
         <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C26">
         <v>2010</v>
       </c>
       <c r="D26" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E26">
         <v>201010</v>
       </c>
       <c r="F26" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G26">
         <v>20101010</v>
       </c>
       <c r="H26" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.45">
@@ -1766,25 +1772,25 @@
         <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C27">
         <v>2010</v>
       </c>
       <c r="D27" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E27">
         <v>201020</v>
       </c>
       <c r="F27" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G27">
         <v>20102010</v>
       </c>
       <c r="H27" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.45">
@@ -1792,25 +1798,25 @@
         <v>20</v>
       </c>
       <c r="B28" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C28">
         <v>2010</v>
       </c>
       <c r="D28" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E28">
         <v>201030</v>
       </c>
       <c r="F28" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G28">
         <v>20103010</v>
       </c>
       <c r="H28" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.45">
@@ -1818,25 +1824,25 @@
         <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C29">
         <v>2010</v>
       </c>
       <c r="D29" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E29">
         <v>201040</v>
       </c>
       <c r="F29" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G29">
         <v>20104010</v>
       </c>
       <c r="H29" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.45">
@@ -1844,25 +1850,25 @@
         <v>20</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C30">
         <v>2010</v>
       </c>
       <c r="D30" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E30">
         <v>201040</v>
       </c>
       <c r="F30" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G30">
         <v>20104020</v>
       </c>
       <c r="H30" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.45">
@@ -1870,25 +1876,25 @@
         <v>20</v>
       </c>
       <c r="B31" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C31">
         <v>2010</v>
       </c>
       <c r="D31" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E31">
         <v>201050</v>
       </c>
       <c r="F31" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G31">
         <v>20105010</v>
       </c>
       <c r="H31" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.45">
@@ -1896,25 +1902,25 @@
         <v>20</v>
       </c>
       <c r="B32" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C32">
         <v>2010</v>
       </c>
       <c r="D32" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E32">
         <v>201060</v>
       </c>
       <c r="F32" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G32">
         <v>20106010</v>
       </c>
       <c r="H32" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.45">
@@ -1922,25 +1928,25 @@
         <v>20</v>
       </c>
       <c r="B33" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C33">
         <v>2010</v>
       </c>
       <c r="D33" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E33">
         <v>201060</v>
       </c>
       <c r="F33" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G33">
         <v>20106015</v>
       </c>
       <c r="H33" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.45">
@@ -1948,25 +1954,25 @@
         <v>20</v>
       </c>
       <c r="B34" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C34">
         <v>2010</v>
       </c>
       <c r="D34" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E34">
         <v>201060</v>
       </c>
       <c r="F34" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G34">
         <v>20106020</v>
       </c>
       <c r="H34" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.45">
@@ -1974,25 +1980,25 @@
         <v>20</v>
       </c>
       <c r="B35" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C35">
         <v>2010</v>
       </c>
       <c r="D35" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E35">
         <v>201070</v>
       </c>
       <c r="F35" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G35">
         <v>20107010</v>
       </c>
       <c r="H35" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.45">
@@ -2000,25 +2006,25 @@
         <v>20</v>
       </c>
       <c r="B36" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C36">
         <v>2020</v>
       </c>
       <c r="D36" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E36">
         <v>202010</v>
       </c>
       <c r="F36" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G36">
         <v>20201010</v>
       </c>
       <c r="H36" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.45">
@@ -2026,25 +2032,25 @@
         <v>20</v>
       </c>
       <c r="B37" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C37">
         <v>2020</v>
       </c>
       <c r="D37" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E37">
         <v>202010</v>
       </c>
       <c r="F37" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G37">
         <v>20201050</v>
       </c>
       <c r="H37" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.45">
@@ -2052,25 +2058,25 @@
         <v>20</v>
       </c>
       <c r="B38" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C38">
         <v>2020</v>
       </c>
       <c r="D38" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E38">
         <v>202010</v>
       </c>
       <c r="F38" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G38">
         <v>20201060</v>
       </c>
       <c r="H38" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.45">
@@ -2078,25 +2084,25 @@
         <v>20</v>
       </c>
       <c r="B39" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C39">
         <v>2020</v>
       </c>
       <c r="D39" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E39">
         <v>202010</v>
       </c>
       <c r="F39" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G39">
         <v>20201070</v>
       </c>
       <c r="H39" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.45">
@@ -2104,25 +2110,25 @@
         <v>20</v>
       </c>
       <c r="B40" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C40">
         <v>2020</v>
       </c>
       <c r="D40" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E40">
         <v>202010</v>
       </c>
       <c r="F40" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="G40">
         <v>20201080</v>
       </c>
       <c r="H40" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.45">
@@ -2130,25 +2136,25 @@
         <v>20</v>
       </c>
       <c r="B41" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C41">
         <v>2020</v>
       </c>
       <c r="D41" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E41">
         <v>202020</v>
       </c>
       <c r="F41" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G41">
         <v>20202010</v>
       </c>
       <c r="H41" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.45">
@@ -2156,25 +2162,25 @@
         <v>20</v>
       </c>
       <c r="B42" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C42">
         <v>2020</v>
       </c>
       <c r="D42" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E42">
         <v>202020</v>
       </c>
       <c r="F42" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G42">
         <v>20202020</v>
       </c>
       <c r="H42" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.45">
@@ -2182,25 +2188,25 @@
         <v>20</v>
       </c>
       <c r="B43" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C43">
         <v>2020</v>
       </c>
       <c r="D43" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E43">
         <v>202020</v>
       </c>
       <c r="F43" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="G43">
         <v>20202030</v>
       </c>
       <c r="H43" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.45">
@@ -2208,25 +2214,25 @@
         <v>20</v>
       </c>
       <c r="B44" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C44">
         <v>2030</v>
       </c>
       <c r="D44" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E44">
         <v>203010</v>
       </c>
       <c r="F44" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G44">
         <v>20301010</v>
       </c>
       <c r="H44" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.45">
@@ -2234,25 +2240,25 @@
         <v>20</v>
       </c>
       <c r="B45" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C45">
         <v>2030</v>
       </c>
       <c r="D45" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E45">
         <v>203020</v>
       </c>
       <c r="F45" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G45">
         <v>20302010</v>
       </c>
       <c r="H45" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.45">
@@ -2260,25 +2266,25 @@
         <v>20</v>
       </c>
       <c r="B46" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C46">
         <v>2030</v>
       </c>
       <c r="D46" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E46">
         <v>203030</v>
       </c>
       <c r="F46" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G46">
         <v>20303010</v>
       </c>
       <c r="H46" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.45">
@@ -2286,25 +2292,25 @@
         <v>20</v>
       </c>
       <c r="B47" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C47">
         <v>2030</v>
       </c>
       <c r="D47" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E47">
         <v>203040</v>
       </c>
       <c r="F47" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G47">
         <v>20304010</v>
       </c>
       <c r="H47" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.45">
@@ -2312,25 +2318,25 @@
         <v>20</v>
       </c>
       <c r="B48" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C48">
         <v>2030</v>
       </c>
       <c r="D48" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E48">
         <v>203040</v>
       </c>
       <c r="F48" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G48">
         <v>20304030</v>
       </c>
       <c r="H48" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.45">
@@ -2338,25 +2344,25 @@
         <v>20</v>
       </c>
       <c r="B49" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C49">
         <v>2030</v>
       </c>
       <c r="D49" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E49">
         <v>203040</v>
       </c>
       <c r="F49" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G49">
         <v>20304040</v>
       </c>
       <c r="H49" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.45">
@@ -2364,25 +2370,25 @@
         <v>20</v>
       </c>
       <c r="B50" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C50">
         <v>2030</v>
       </c>
       <c r="D50" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E50">
         <v>203050</v>
       </c>
       <c r="F50" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G50">
         <v>20305010</v>
       </c>
       <c r="H50" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.45">
@@ -2390,25 +2396,25 @@
         <v>20</v>
       </c>
       <c r="B51" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C51">
         <v>2030</v>
       </c>
       <c r="D51" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E51">
         <v>203050</v>
       </c>
       <c r="F51" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G51">
         <v>20305020</v>
       </c>
       <c r="H51" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.45">
@@ -2416,25 +2422,25 @@
         <v>20</v>
       </c>
       <c r="B52" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C52">
         <v>2030</v>
       </c>
       <c r="D52" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E52">
         <v>203050</v>
       </c>
       <c r="F52" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G52">
         <v>20305030</v>
       </c>
       <c r="H52" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.45">
@@ -2442,25 +2448,25 @@
         <v>25</v>
       </c>
       <c r="B53" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C53">
         <v>2510</v>
       </c>
       <c r="D53" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E53">
         <v>251010</v>
       </c>
       <c r="F53" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G53">
         <v>25101010</v>
       </c>
       <c r="H53" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.45">
@@ -2468,25 +2474,25 @@
         <v>25</v>
       </c>
       <c r="B54" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C54">
         <v>2510</v>
       </c>
       <c r="D54" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E54">
         <v>251010</v>
       </c>
       <c r="F54" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="G54">
         <v>25101020</v>
       </c>
       <c r="H54" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.45">
@@ -2494,25 +2500,25 @@
         <v>25</v>
       </c>
       <c r="B55" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C55">
         <v>2510</v>
       </c>
       <c r="D55" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E55">
         <v>251020</v>
       </c>
       <c r="F55" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G55">
         <v>25102010</v>
       </c>
       <c r="H55" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.45">
@@ -2520,25 +2526,25 @@
         <v>25</v>
       </c>
       <c r="B56" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C56">
         <v>2510</v>
       </c>
       <c r="D56" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E56">
         <v>251020</v>
       </c>
       <c r="F56" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G56">
         <v>25102020</v>
       </c>
       <c r="H56" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.45">
@@ -2546,25 +2552,25 @@
         <v>25</v>
       </c>
       <c r="B57" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C57">
         <v>2520</v>
       </c>
       <c r="D57" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E57">
         <v>252010</v>
       </c>
       <c r="F57" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G57">
         <v>25201010</v>
       </c>
       <c r="H57" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.45">
@@ -2572,25 +2578,25 @@
         <v>25</v>
       </c>
       <c r="B58" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C58">
         <v>2520</v>
       </c>
       <c r="D58" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E58">
         <v>252010</v>
       </c>
       <c r="F58" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G58">
         <v>25201020</v>
       </c>
       <c r="H58" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.45">
@@ -2598,25 +2604,25 @@
         <v>25</v>
       </c>
       <c r="B59" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C59">
         <v>2520</v>
       </c>
       <c r="D59" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E59">
         <v>252010</v>
       </c>
       <c r="F59" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G59">
         <v>25201030</v>
       </c>
       <c r="H59" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.45">
@@ -2624,25 +2630,25 @@
         <v>25</v>
       </c>
       <c r="B60" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C60">
         <v>2520</v>
       </c>
       <c r="D60" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E60">
         <v>252010</v>
       </c>
       <c r="F60" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G60">
         <v>25201040</v>
       </c>
       <c r="H60" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.45">
@@ -2650,25 +2656,25 @@
         <v>25</v>
       </c>
       <c r="B61" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C61">
         <v>2520</v>
       </c>
       <c r="D61" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E61">
         <v>252010</v>
       </c>
       <c r="F61" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G61">
         <v>25201050</v>
       </c>
       <c r="H61" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.45">
@@ -2676,25 +2682,25 @@
         <v>25</v>
       </c>
       <c r="B62" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C62">
         <v>2520</v>
       </c>
       <c r="D62" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E62">
         <v>252020</v>
       </c>
       <c r="F62" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="G62">
         <v>25202010</v>
       </c>
       <c r="H62" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -2702,25 +2708,25 @@
         <v>25</v>
       </c>
       <c r="B63" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C63">
         <v>2520</v>
       </c>
       <c r="D63" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E63">
         <v>252030</v>
       </c>
       <c r="F63" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G63">
         <v>25203010</v>
       </c>
       <c r="H63" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.45">
@@ -2728,25 +2734,25 @@
         <v>25</v>
       </c>
       <c r="B64" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C64">
         <v>2520</v>
       </c>
       <c r="D64" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E64">
         <v>252030</v>
       </c>
       <c r="F64" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G64">
         <v>25203020</v>
       </c>
       <c r="H64" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.45">
@@ -2754,25 +2760,25 @@
         <v>25</v>
       </c>
       <c r="B65" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C65">
         <v>2520</v>
       </c>
       <c r="D65" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E65">
         <v>252030</v>
       </c>
       <c r="F65" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G65">
         <v>25203030</v>
       </c>
       <c r="H65" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.45">
@@ -2780,25 +2786,25 @@
         <v>25</v>
       </c>
       <c r="B66" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C66">
         <v>2530</v>
       </c>
       <c r="D66" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E66">
         <v>253010</v>
       </c>
       <c r="F66" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G66">
         <v>25301010</v>
       </c>
       <c r="H66" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.45">
@@ -2806,25 +2812,25 @@
         <v>25</v>
       </c>
       <c r="B67" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C67">
         <v>2530</v>
       </c>
       <c r="D67" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E67">
         <v>253010</v>
       </c>
       <c r="F67" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G67">
         <v>25301020</v>
       </c>
       <c r="H67" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.45">
@@ -2832,25 +2838,25 @@
         <v>25</v>
       </c>
       <c r="B68" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C68">
         <v>2530</v>
       </c>
       <c r="D68" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E68">
         <v>253010</v>
       </c>
       <c r="F68" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G68">
         <v>25301030</v>
       </c>
       <c r="H68" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.45">
@@ -2858,25 +2864,25 @@
         <v>25</v>
       </c>
       <c r="B69" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C69">
         <v>2530</v>
       </c>
       <c r="D69" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E69">
         <v>253010</v>
       </c>
       <c r="F69" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G69">
         <v>25301040</v>
       </c>
       <c r="H69" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.45">
@@ -2884,25 +2890,25 @@
         <v>25</v>
       </c>
       <c r="B70" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C70">
         <v>2530</v>
       </c>
       <c r="D70" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E70">
         <v>253020</v>
       </c>
       <c r="F70" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G70">
         <v>25302010</v>
       </c>
       <c r="H70" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.45">
@@ -2910,25 +2916,25 @@
         <v>25</v>
       </c>
       <c r="B71" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C71">
         <v>2530</v>
       </c>
       <c r="D71" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E71">
         <v>253020</v>
       </c>
       <c r="F71" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G71">
         <v>25302020</v>
       </c>
       <c r="H71" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.45">
@@ -2936,25 +2942,25 @@
         <v>25</v>
       </c>
       <c r="B72" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C72">
         <v>2550</v>
       </c>
       <c r="D72" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E72">
         <v>255010</v>
       </c>
       <c r="F72" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G72">
         <v>25501010</v>
       </c>
       <c r="H72" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.45">
@@ -2962,25 +2968,25 @@
         <v>25</v>
       </c>
       <c r="B73" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C73">
         <v>2550</v>
       </c>
       <c r="D73" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E73">
         <v>255030</v>
       </c>
       <c r="F73" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="G73">
         <v>25503030</v>
       </c>
       <c r="H73" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.45">
@@ -2988,25 +2994,25 @@
         <v>25</v>
       </c>
       <c r="B74" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C74">
         <v>2550</v>
       </c>
       <c r="D74" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E74">
         <v>255040</v>
       </c>
       <c r="F74" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G74">
         <v>25504010</v>
       </c>
       <c r="H74" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.45">
@@ -3014,25 +3020,25 @@
         <v>25</v>
       </c>
       <c r="B75" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C75">
         <v>2550</v>
       </c>
       <c r="D75" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E75">
         <v>255040</v>
       </c>
       <c r="F75" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G75">
         <v>25504020</v>
       </c>
       <c r="H75" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.45">
@@ -3040,25 +3046,25 @@
         <v>25</v>
       </c>
       <c r="B76" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C76">
         <v>2550</v>
       </c>
       <c r="D76" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E76">
         <v>255040</v>
       </c>
       <c r="F76" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G76">
         <v>25504030</v>
       </c>
       <c r="H76" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.45">
@@ -3066,25 +3072,25 @@
         <v>25</v>
       </c>
       <c r="B77" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C77">
         <v>2550</v>
       </c>
       <c r="D77" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E77">
         <v>255040</v>
       </c>
       <c r="F77" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G77">
         <v>25504040</v>
       </c>
       <c r="H77" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.45">
@@ -3092,25 +3098,25 @@
         <v>25</v>
       </c>
       <c r="B78" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C78">
         <v>2550</v>
       </c>
       <c r="D78" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E78">
         <v>255040</v>
       </c>
       <c r="F78" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G78">
         <v>25504050</v>
       </c>
       <c r="H78" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.45">
@@ -3118,25 +3124,25 @@
         <v>25</v>
       </c>
       <c r="B79" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C79">
         <v>2550</v>
       </c>
       <c r="D79" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E79">
         <v>255040</v>
       </c>
       <c r="F79" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="G79">
         <v>25504060</v>
       </c>
       <c r="H79" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.45">
@@ -3144,25 +3150,25 @@
         <v>30</v>
       </c>
       <c r="B80" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C80">
         <v>3010</v>
       </c>
       <c r="D80" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E80">
         <v>301010</v>
       </c>
       <c r="F80" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G80">
         <v>30101010</v>
       </c>
       <c r="H80" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.45">
@@ -3170,25 +3176,25 @@
         <v>30</v>
       </c>
       <c r="B81" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C81">
         <v>3010</v>
       </c>
       <c r="D81" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E81">
         <v>301010</v>
       </c>
       <c r="F81" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G81">
         <v>30101020</v>
       </c>
       <c r="H81" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.45">
@@ -3196,25 +3202,25 @@
         <v>30</v>
       </c>
       <c r="B82" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C82">
         <v>3010</v>
       </c>
       <c r="D82" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E82">
         <v>301010</v>
       </c>
       <c r="F82" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G82">
         <v>30101030</v>
       </c>
       <c r="H82" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.45">
@@ -3222,25 +3228,25 @@
         <v>30</v>
       </c>
       <c r="B83" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C83">
         <v>3010</v>
       </c>
       <c r="D83" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E83">
         <v>301010</v>
       </c>
       <c r="F83" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G83">
         <v>30101040</v>
       </c>
       <c r="H83" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.45">
@@ -3248,25 +3254,25 @@
         <v>30</v>
       </c>
       <c r="B84" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C84">
         <v>3020</v>
       </c>
       <c r="D84" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E84">
         <v>302010</v>
       </c>
       <c r="F84" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="G84">
         <v>30201010</v>
       </c>
       <c r="H84" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.45">
@@ -3274,25 +3280,25 @@
         <v>30</v>
       </c>
       <c r="B85" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C85">
         <v>3020</v>
       </c>
       <c r="D85" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E85">
         <v>302010</v>
       </c>
       <c r="F85" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="G85">
         <v>30201020</v>
       </c>
       <c r="H85" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.45">
@@ -3300,25 +3306,25 @@
         <v>30</v>
       </c>
       <c r="B86" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C86">
         <v>3020</v>
       </c>
       <c r="D86" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E86">
         <v>302010</v>
       </c>
       <c r="F86" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="G86">
         <v>30201030</v>
       </c>
       <c r="H86" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.45">
@@ -3326,25 +3332,25 @@
         <v>30</v>
       </c>
       <c r="B87" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C87">
         <v>3020</v>
       </c>
       <c r="D87" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E87">
         <v>302020</v>
       </c>
       <c r="F87" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="G87">
         <v>30202010</v>
       </c>
       <c r="H87" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.45">
@@ -3352,25 +3358,25 @@
         <v>30</v>
       </c>
       <c r="B88" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C88">
         <v>3020</v>
       </c>
       <c r="D88" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E88">
         <v>302020</v>
       </c>
       <c r="F88" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="G88">
         <v>30202030</v>
       </c>
       <c r="H88" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.45">
@@ -3378,25 +3384,25 @@
         <v>30</v>
       </c>
       <c r="B89" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C89">
         <v>3020</v>
       </c>
       <c r="D89" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E89">
         <v>302030</v>
       </c>
       <c r="F89" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G89">
         <v>30203010</v>
       </c>
       <c r="H89" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.45">
@@ -3404,25 +3410,25 @@
         <v>30</v>
       </c>
       <c r="B90" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C90">
         <v>3030</v>
       </c>
       <c r="D90" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E90">
         <v>303010</v>
       </c>
       <c r="F90" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G90">
         <v>30301010</v>
       </c>
       <c r="H90" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.45">
@@ -3430,25 +3436,25 @@
         <v>30</v>
       </c>
       <c r="B91" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C91">
         <v>3030</v>
       </c>
       <c r="D91" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E91">
         <v>303020</v>
       </c>
       <c r="F91" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="G91">
         <v>30302010</v>
       </c>
       <c r="H91" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.45">
@@ -3456,25 +3462,25 @@
         <v>35</v>
       </c>
       <c r="B92" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C92">
         <v>3510</v>
       </c>
       <c r="D92" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E92">
         <v>351010</v>
       </c>
       <c r="F92" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G92">
         <v>35101010</v>
       </c>
       <c r="H92" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.45">
@@ -3482,25 +3488,25 @@
         <v>35</v>
       </c>
       <c r="B93" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C93">
         <v>3510</v>
       </c>
       <c r="D93" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E93">
         <v>351010</v>
       </c>
       <c r="F93" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G93">
         <v>35101020</v>
       </c>
       <c r="H93" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.45">
@@ -3508,25 +3514,25 @@
         <v>35</v>
       </c>
       <c r="B94" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C94">
         <v>3510</v>
       </c>
       <c r="D94" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E94">
         <v>351020</v>
       </c>
       <c r="F94" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="G94">
         <v>35102010</v>
       </c>
       <c r="H94" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.45">
@@ -3534,25 +3540,25 @@
         <v>35</v>
       </c>
       <c r="B95" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C95">
         <v>3510</v>
       </c>
       <c r="D95" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E95">
         <v>351020</v>
       </c>
       <c r="F95" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="G95">
         <v>35102015</v>
       </c>
       <c r="H95" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.45">
@@ -3560,25 +3566,25 @@
         <v>35</v>
       </c>
       <c r="B96" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C96">
         <v>3510</v>
       </c>
       <c r="D96" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E96">
         <v>351020</v>
       </c>
       <c r="F96" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="G96">
         <v>35102020</v>
       </c>
       <c r="H96" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.45">
@@ -3586,25 +3592,25 @@
         <v>35</v>
       </c>
       <c r="B97" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C97">
         <v>3510</v>
       </c>
       <c r="D97" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E97">
         <v>351020</v>
       </c>
       <c r="F97" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="G97">
         <v>35102030</v>
       </c>
       <c r="H97" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.45">
@@ -3612,25 +3618,25 @@
         <v>35</v>
       </c>
       <c r="B98" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C98">
         <v>3510</v>
       </c>
       <c r="D98" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E98">
         <v>351030</v>
       </c>
       <c r="F98" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G98">
         <v>35103010</v>
       </c>
       <c r="H98" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.45">
@@ -3638,25 +3644,25 @@
         <v>35</v>
       </c>
       <c r="B99" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C99">
         <v>3520</v>
       </c>
       <c r="D99" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E99">
         <v>352010</v>
       </c>
       <c r="F99" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G99">
         <v>35201010</v>
       </c>
       <c r="H99" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.45">
@@ -3664,25 +3670,25 @@
         <v>35</v>
       </c>
       <c r="B100" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C100">
         <v>3520</v>
       </c>
       <c r="D100" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E100">
         <v>352020</v>
       </c>
       <c r="F100" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="G100">
         <v>35202010</v>
       </c>
       <c r="H100" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.45">
@@ -3690,25 +3696,25 @@
         <v>35</v>
       </c>
       <c r="B101" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C101">
         <v>3520</v>
       </c>
       <c r="D101" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E101">
         <v>352030</v>
       </c>
       <c r="F101" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G101">
         <v>35203010</v>
       </c>
       <c r="H101" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.45">
@@ -3716,25 +3722,25 @@
         <v>40</v>
       </c>
       <c r="B102" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C102">
         <v>4010</v>
       </c>
       <c r="D102" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E102">
         <v>401010</v>
       </c>
       <c r="F102" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="G102">
         <v>40101010</v>
       </c>
       <c r="H102" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.45">
@@ -3742,25 +3748,25 @@
         <v>40</v>
       </c>
       <c r="B103" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C103">
         <v>4010</v>
       </c>
       <c r="D103" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E103">
         <v>401010</v>
       </c>
       <c r="F103" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="G103">
         <v>40101015</v>
       </c>
       <c r="H103" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.45">
@@ -3768,25 +3774,25 @@
         <v>40</v>
       </c>
       <c r="B104" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C104">
         <v>4020</v>
       </c>
       <c r="D104" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E104">
         <v>402010</v>
       </c>
       <c r="F104" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G104">
         <v>40201020</v>
       </c>
       <c r="H104" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.45">
@@ -3794,25 +3800,25 @@
         <v>40</v>
       </c>
       <c r="B105" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C105">
         <v>4020</v>
       </c>
       <c r="D105" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E105">
         <v>402010</v>
       </c>
       <c r="F105" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G105">
         <v>40201030</v>
       </c>
       <c r="H105" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.45">
@@ -3820,25 +3826,25 @@
         <v>40</v>
       </c>
       <c r="B106" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C106">
         <v>4020</v>
       </c>
       <c r="D106" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E106">
         <v>402010</v>
       </c>
       <c r="F106" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G106">
         <v>40201040</v>
       </c>
       <c r="H106" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.45">
@@ -3846,25 +3852,25 @@
         <v>40</v>
       </c>
       <c r="B107" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C107">
         <v>4020</v>
       </c>
       <c r="D107" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E107">
         <v>402010</v>
       </c>
       <c r="F107" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G107">
         <v>40201050</v>
       </c>
       <c r="H107" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.45">
@@ -3872,25 +3878,25 @@
         <v>40</v>
       </c>
       <c r="B108" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C108">
         <v>4020</v>
       </c>
       <c r="D108" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E108">
         <v>402010</v>
       </c>
       <c r="F108" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G108">
         <v>40201060</v>
       </c>
       <c r="H108" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.45">
@@ -3898,25 +3904,25 @@
         <v>40</v>
       </c>
       <c r="B109" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C109">
         <v>4020</v>
       </c>
       <c r="D109" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E109">
         <v>402020</v>
       </c>
       <c r="F109" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="G109">
         <v>40202010</v>
       </c>
       <c r="H109" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.45">
@@ -3924,25 +3930,25 @@
         <v>40</v>
       </c>
       <c r="B110" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C110">
         <v>4020</v>
       </c>
       <c r="D110" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E110">
         <v>402030</v>
       </c>
       <c r="F110" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G110">
         <v>40203010</v>
       </c>
       <c r="H110" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.45">
@@ -3950,25 +3956,25 @@
         <v>40</v>
       </c>
       <c r="B111" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C111">
         <v>4020</v>
       </c>
       <c r="D111" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E111">
         <v>402030</v>
       </c>
       <c r="F111" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G111">
         <v>40203020</v>
       </c>
       <c r="H111" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.45">
@@ -3976,25 +3982,25 @@
         <v>40</v>
       </c>
       <c r="B112" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C112">
         <v>4020</v>
       </c>
       <c r="D112" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E112">
         <v>402030</v>
       </c>
       <c r="F112" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G112">
         <v>40203030</v>
       </c>
       <c r="H112" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.45">
@@ -4002,25 +4008,25 @@
         <v>40</v>
       </c>
       <c r="B113" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C113">
         <v>4020</v>
       </c>
       <c r="D113" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E113">
         <v>402030</v>
       </c>
       <c r="F113" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G113">
         <v>40203040</v>
       </c>
       <c r="H113" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.45">
@@ -4028,25 +4034,25 @@
         <v>40</v>
       </c>
       <c r="B114" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C114">
         <v>4020</v>
       </c>
       <c r="D114" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E114">
         <v>402040</v>
       </c>
       <c r="F114" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G114">
         <v>40204010</v>
       </c>
       <c r="H114" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.45">
@@ -4054,25 +4060,25 @@
         <v>40</v>
       </c>
       <c r="B115" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C115">
         <v>4030</v>
       </c>
       <c r="D115" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E115">
         <v>403010</v>
       </c>
       <c r="F115" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="G115">
         <v>40301010</v>
       </c>
       <c r="H115" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.45">
@@ -4080,25 +4086,25 @@
         <v>40</v>
       </c>
       <c r="B116" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C116">
         <v>4030</v>
       </c>
       <c r="D116" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E116">
         <v>403010</v>
       </c>
       <c r="F116" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="G116">
         <v>40301020</v>
       </c>
       <c r="H116" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.45">
@@ -4106,25 +4112,25 @@
         <v>40</v>
       </c>
       <c r="B117" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C117">
         <v>4030</v>
       </c>
       <c r="D117" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E117">
         <v>403010</v>
       </c>
       <c r="F117" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="G117">
         <v>40301030</v>
       </c>
       <c r="H117" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.45">
@@ -4132,25 +4138,25 @@
         <v>40</v>
       </c>
       <c r="B118" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C118">
         <v>4030</v>
       </c>
       <c r="D118" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E118">
         <v>403010</v>
       </c>
       <c r="F118" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="G118">
         <v>40301040</v>
       </c>
       <c r="H118" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.45">
@@ -4158,25 +4164,25 @@
         <v>40</v>
       </c>
       <c r="B119" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C119">
         <v>4030</v>
       </c>
       <c r="D119" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E119">
         <v>403010</v>
       </c>
       <c r="F119" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="G119">
         <v>40301050</v>
       </c>
       <c r="H119" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.45">
@@ -4184,25 +4190,25 @@
         <v>45</v>
       </c>
       <c r="B120" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C120">
         <v>4510</v>
       </c>
       <c r="D120" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E120">
         <v>451020</v>
       </c>
       <c r="F120" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="G120">
         <v>45102010</v>
       </c>
       <c r="H120" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.45">
@@ -4210,25 +4216,25 @@
         <v>45</v>
       </c>
       <c r="B121" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C121">
         <v>4510</v>
       </c>
       <c r="D121" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E121">
         <v>451020</v>
       </c>
       <c r="F121" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="G121">
         <v>45102030</v>
       </c>
       <c r="H121" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.45">
@@ -4236,25 +4242,25 @@
         <v>45</v>
       </c>
       <c r="B122" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C122">
         <v>4510</v>
       </c>
       <c r="D122" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E122">
         <v>451030</v>
       </c>
       <c r="F122" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="G122">
         <v>45103010</v>
       </c>
       <c r="H122" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.45">
@@ -4262,25 +4268,25 @@
         <v>45</v>
       </c>
       <c r="B123" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C123">
         <v>4510</v>
       </c>
       <c r="D123" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E123">
         <v>451030</v>
       </c>
       <c r="F123" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="G123">
         <v>45103020</v>
       </c>
       <c r="H123" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.45">
@@ -4288,25 +4294,25 @@
         <v>45</v>
       </c>
       <c r="B124" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C124">
         <v>4520</v>
       </c>
       <c r="D124" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E124">
         <v>452010</v>
       </c>
       <c r="F124" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="G124">
         <v>45201020</v>
       </c>
       <c r="H124" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.45">
@@ -4314,25 +4320,25 @@
         <v>45</v>
       </c>
       <c r="B125" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C125">
         <v>4520</v>
       </c>
       <c r="D125" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E125">
         <v>452020</v>
       </c>
       <c r="F125" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="G125">
         <v>45202030</v>
       </c>
       <c r="H125" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.45">
@@ -4340,25 +4346,25 @@
         <v>45</v>
       </c>
       <c r="B126" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C126">
         <v>4520</v>
       </c>
       <c r="D126" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E126">
         <v>452030</v>
       </c>
       <c r="F126" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="G126">
         <v>45203010</v>
       </c>
       <c r="H126" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.45">
@@ -4366,25 +4372,25 @@
         <v>45</v>
       </c>
       <c r="B127" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C127">
         <v>4520</v>
       </c>
       <c r="D127" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E127">
         <v>452030</v>
       </c>
       <c r="F127" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="G127">
         <v>45203015</v>
       </c>
       <c r="H127" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.45">
@@ -4392,25 +4398,25 @@
         <v>45</v>
       </c>
       <c r="B128" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C128">
         <v>4520</v>
       </c>
       <c r="D128" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E128">
         <v>452030</v>
       </c>
       <c r="F128" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="G128">
         <v>45203020</v>
       </c>
       <c r="H128" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.45">
@@ -4418,25 +4424,25 @@
         <v>45</v>
       </c>
       <c r="B129" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C129">
         <v>4520</v>
       </c>
       <c r="D129" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E129">
         <v>452030</v>
       </c>
       <c r="F129" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="G129">
         <v>45203030</v>
       </c>
       <c r="H129" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.45">
@@ -4444,25 +4450,25 @@
         <v>45</v>
       </c>
       <c r="B130" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C130">
         <v>4530</v>
       </c>
       <c r="D130" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E130">
         <v>453010</v>
       </c>
       <c r="F130" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="G130">
         <v>45301010</v>
       </c>
       <c r="H130" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.45">
@@ -4470,25 +4476,25 @@
         <v>45</v>
       </c>
       <c r="B131" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C131">
         <v>4530</v>
       </c>
       <c r="D131" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E131">
         <v>453010</v>
       </c>
       <c r="F131" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="G131">
         <v>45301020</v>
       </c>
       <c r="H131" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.45">
@@ -4496,25 +4502,25 @@
         <v>50</v>
       </c>
       <c r="B132" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C132">
         <v>5010</v>
       </c>
       <c r="D132" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E132">
         <v>501010</v>
       </c>
       <c r="F132" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="G132">
         <v>50101010</v>
       </c>
       <c r="H132" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.45">
@@ -4522,25 +4528,25 @@
         <v>50</v>
       </c>
       <c r="B133" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C133">
         <v>5010</v>
       </c>
       <c r="D133" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E133">
         <v>501010</v>
       </c>
       <c r="F133" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="G133">
         <v>50101020</v>
       </c>
       <c r="H133" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.45">
@@ -4548,25 +4554,25 @@
         <v>50</v>
       </c>
       <c r="B134" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C134">
         <v>5010</v>
       </c>
       <c r="D134" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E134">
         <v>501020</v>
       </c>
       <c r="F134" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="G134">
         <v>50102010</v>
       </c>
       <c r="H134" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.45">
@@ -4574,25 +4580,25 @@
         <v>50</v>
       </c>
       <c r="B135" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C135">
         <v>5020</v>
       </c>
       <c r="D135" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E135">
         <v>502010</v>
       </c>
       <c r="F135" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="G135">
         <v>50201010</v>
       </c>
       <c r="H135" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.45">
@@ -4600,25 +4606,25 @@
         <v>50</v>
       </c>
       <c r="B136" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C136">
         <v>5020</v>
       </c>
       <c r="D136" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E136">
         <v>502010</v>
       </c>
       <c r="F136" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="G136">
         <v>50201020</v>
       </c>
       <c r="H136" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.45">
@@ -4626,25 +4632,25 @@
         <v>50</v>
       </c>
       <c r="B137" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C137">
         <v>5020</v>
       </c>
       <c r="D137" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E137">
         <v>502010</v>
       </c>
       <c r="F137" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="G137">
         <v>50201030</v>
       </c>
       <c r="H137" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.45">
@@ -4652,25 +4658,25 @@
         <v>50</v>
       </c>
       <c r="B138" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C138">
         <v>5020</v>
       </c>
       <c r="D138" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E138">
         <v>502010</v>
       </c>
       <c r="F138" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="G138">
         <v>50201040</v>
       </c>
       <c r="H138" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.45">
@@ -4678,25 +4684,25 @@
         <v>50</v>
       </c>
       <c r="B139" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C139">
         <v>5020</v>
       </c>
       <c r="D139" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E139">
         <v>502020</v>
       </c>
       <c r="F139" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="G139">
         <v>50202010</v>
       </c>
       <c r="H139" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.45">
@@ -4704,25 +4710,25 @@
         <v>50</v>
       </c>
       <c r="B140" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C140">
         <v>5020</v>
       </c>
       <c r="D140" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E140">
         <v>502020</v>
       </c>
       <c r="F140" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="G140">
         <v>50202020</v>
       </c>
       <c r="H140" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.45">
@@ -4730,25 +4736,25 @@
         <v>50</v>
       </c>
       <c r="B141" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C141">
         <v>5020</v>
       </c>
       <c r="D141" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E141">
         <v>502030</v>
       </c>
       <c r="F141" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="G141">
         <v>50203010</v>
       </c>
       <c r="H141" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.45">
@@ -4756,25 +4762,25 @@
         <v>55</v>
       </c>
       <c r="B142" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C142">
         <v>5510</v>
       </c>
       <c r="D142" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E142">
         <v>551010</v>
       </c>
       <c r="F142" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="G142">
         <v>55101010</v>
       </c>
       <c r="H142" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.45">
@@ -4782,25 +4788,25 @@
         <v>55</v>
       </c>
       <c r="B143" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C143">
         <v>5510</v>
       </c>
       <c r="D143" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E143">
         <v>551020</v>
       </c>
       <c r="F143" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="G143">
         <v>55102010</v>
       </c>
       <c r="H143" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.45">
@@ -4808,25 +4814,25 @@
         <v>55</v>
       </c>
       <c r="B144" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C144">
         <v>5510</v>
       </c>
       <c r="D144" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E144">
         <v>551030</v>
       </c>
       <c r="F144" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="G144">
         <v>55103010</v>
       </c>
       <c r="H144" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.45">
@@ -4834,25 +4840,25 @@
         <v>55</v>
       </c>
       <c r="B145" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C145">
         <v>5510</v>
       </c>
       <c r="D145" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E145">
         <v>551040</v>
       </c>
       <c r="F145" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G145">
         <v>55104010</v>
       </c>
       <c r="H145" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.45">
@@ -4860,25 +4866,25 @@
         <v>55</v>
       </c>
       <c r="B146" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C146">
         <v>5510</v>
       </c>
       <c r="D146" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E146">
         <v>551050</v>
       </c>
       <c r="F146" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="G146">
         <v>55105010</v>
       </c>
       <c r="H146" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.45">
@@ -4886,25 +4892,25 @@
         <v>55</v>
       </c>
       <c r="B147" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C147">
         <v>5510</v>
       </c>
       <c r="D147" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E147">
         <v>551050</v>
       </c>
       <c r="F147" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="G147">
         <v>55105020</v>
       </c>
       <c r="H147" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.45">
@@ -4912,25 +4918,25 @@
         <v>60</v>
       </c>
       <c r="B148" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C148">
         <v>6010</v>
       </c>
       <c r="D148" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E148">
         <v>601010</v>
       </c>
       <c r="F148" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="G148">
         <v>60101010</v>
       </c>
       <c r="H148" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.45">
@@ -4938,25 +4944,25 @@
         <v>60</v>
       </c>
       <c r="B149" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C149">
         <v>6010</v>
       </c>
       <c r="D149" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E149">
         <v>601025</v>
       </c>
       <c r="F149" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="G149">
         <v>60102510</v>
       </c>
       <c r="H149" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.45">
@@ -4964,25 +4970,25 @@
         <v>60</v>
       </c>
       <c r="B150" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C150">
         <v>6010</v>
       </c>
       <c r="D150" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E150">
         <v>601030</v>
       </c>
       <c r="F150" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="G150">
         <v>60103010</v>
       </c>
       <c r="H150" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.45">
@@ -4990,25 +4996,25 @@
         <v>60</v>
       </c>
       <c r="B151" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C151">
         <v>6010</v>
       </c>
       <c r="D151" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E151">
         <v>601040</v>
       </c>
       <c r="F151" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="G151">
         <v>60104010</v>
       </c>
       <c r="H151" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.45">
@@ -5016,25 +5022,25 @@
         <v>60</v>
       </c>
       <c r="B152" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C152">
         <v>6010</v>
       </c>
       <c r="D152" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E152">
         <v>601050</v>
       </c>
       <c r="F152" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="G152">
         <v>60105010</v>
       </c>
       <c r="H152" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.45">
@@ -5042,25 +5048,25 @@
         <v>60</v>
       </c>
       <c r="B153" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C153">
         <v>6010</v>
       </c>
       <c r="D153" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E153">
         <v>601060</v>
       </c>
       <c r="F153" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G153">
         <v>60106010</v>
       </c>
       <c r="H153" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.45">
@@ -5068,25 +5074,25 @@
         <v>60</v>
       </c>
       <c r="B154" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C154">
         <v>6010</v>
       </c>
       <c r="D154" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E154">
         <v>601060</v>
       </c>
       <c r="F154" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G154">
         <v>60106020</v>
       </c>
       <c r="H154" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.45">
@@ -5094,25 +5100,25 @@
         <v>60</v>
       </c>
       <c r="B155" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C155">
         <v>6010</v>
       </c>
       <c r="D155" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E155">
         <v>601070</v>
       </c>
       <c r="F155" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="G155">
         <v>60107010</v>
       </c>
       <c r="H155" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.45">
@@ -5120,25 +5126,25 @@
         <v>60</v>
       </c>
       <c r="B156" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C156">
         <v>6010</v>
       </c>
       <c r="D156" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E156">
         <v>601080</v>
       </c>
       <c r="F156" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G156">
         <v>60108010</v>
       </c>
       <c r="H156" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.45">
@@ -5146,25 +5152,25 @@
         <v>60</v>
       </c>
       <c r="B157" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C157">
         <v>6010</v>
       </c>
       <c r="D157" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E157">
         <v>601080</v>
       </c>
       <c r="F157" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G157">
         <v>60108020</v>
       </c>
       <c r="H157" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.45">
@@ -5172,25 +5178,25 @@
         <v>60</v>
       </c>
       <c r="B158" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C158">
         <v>6010</v>
       </c>
       <c r="D158" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E158">
         <v>601080</v>
       </c>
       <c r="F158" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G158">
         <v>60108030</v>
       </c>
       <c r="H158" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.45">
@@ -5198,25 +5204,25 @@
         <v>60</v>
       </c>
       <c r="B159" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C159">
         <v>6010</v>
       </c>
       <c r="D159" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E159">
         <v>601080</v>
       </c>
       <c r="F159" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G159">
         <v>60108040</v>
       </c>
       <c r="H159" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.45">
@@ -5224,25 +5230,25 @@
         <v>60</v>
       </c>
       <c r="B160" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C160">
         <v>6010</v>
       </c>
       <c r="D160" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E160">
         <v>601080</v>
       </c>
       <c r="F160" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G160">
         <v>60108050</v>
       </c>
       <c r="H160" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.45">
@@ -5250,25 +5256,25 @@
         <v>60</v>
       </c>
       <c r="B161" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C161">
         <v>6020</v>
       </c>
       <c r="D161" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E161">
         <v>602010</v>
       </c>
       <c r="F161" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="G161">
         <v>60201010</v>
       </c>
       <c r="H161" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.45">
@@ -5276,25 +5282,25 @@
         <v>60</v>
       </c>
       <c r="B162" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C162">
         <v>6020</v>
       </c>
       <c r="D162" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E162">
         <v>602010</v>
       </c>
       <c r="F162" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="G162">
         <v>60201020</v>
       </c>
       <c r="H162" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.45">
@@ -5302,25 +5308,25 @@
         <v>60</v>
       </c>
       <c r="B163" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C163">
         <v>6020</v>
       </c>
       <c r="D163" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E163">
         <v>602010</v>
       </c>
       <c r="F163" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="G163">
         <v>60201030</v>
       </c>
       <c r="H163" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.45">
@@ -5328,25 +5334,25 @@
         <v>60</v>
       </c>
       <c r="B164" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C164">
         <v>6020</v>
       </c>
       <c r="D164" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E164">
         <v>602010</v>
       </c>
       <c r="F164" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="G164">
         <v>60201040</v>
       </c>
       <c r="H164" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>